<commit_message>
Small edits/layout changes to publication summary table
</commit_message>
<xml_diff>
--- a/data/publication_summary.xlsx
+++ b/data/publication_summary.xlsx
@@ -216,12 +216,6 @@
     <t>Sikora, Delane, and Delaney (2013b)</t>
   </si>
   <si>
-    <t>Sikora, Lawrence, and Gutierrez-Estrada et al., "Ballad," (2005)</t>
-  </si>
-  <si>
-    <t>Sikora, Lawrence, and Gutierrez-Estrada et al., "Asian soybean rust," (2005)</t>
-  </si>
-  <si>
     <t>Mueller, Miles, and Hartman (2008)</t>
   </si>
   <si>
@@ -247,6 +241,12 @@
   </si>
   <si>
     <t>Lawrence et al., "Punch and Charisma 2006," (2006)</t>
+  </si>
+  <si>
+    <t>Sikora, et al., "Asian soybean rust," (2005)</t>
+  </si>
+  <si>
+    <t>Sikora,et al., "Ballad," (2005)</t>
   </si>
 </sst>
 </file>
@@ -307,8 +307,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -364,7 +430,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -385,6 +451,39 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +504,39 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -737,20 +869,21 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A62" sqref="A55:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -771,408 +904,451 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>8</v>
       </c>
       <c r="F2" s="2">
-        <v>71</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="6" t="s">
-        <v>74</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="6" t="s">
-        <v>47</v>
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2">
-        <v>70</v>
+        <v>14</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1">
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2010</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2011</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>13</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2011</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>14</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2013</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1">
-        <v>9</v>
-      </c>
-      <c r="F11" s="2">
-        <v>31</v>
-      </c>
-      <c r="G11"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2013</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="4">
-        <v>9</v>
-      </c>
-      <c r="F12" s="5">
-        <v>30</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2">
-        <v>6</v>
-      </c>
-      <c r="G13"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15" s="2">
-        <v>67</v>
+        <v>24</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2">
+        <v>31</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>30</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1">
         <v>2008</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E19" s="1">
         <v>18</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F19" s="2">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
         <v>2008</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E20" s="1">
         <v>13</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F20" s="2">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2006</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="4">
-        <v>12</v>
-      </c>
-      <c r="F18" s="5">
-        <v>47</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2006</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="4">
-        <v>12</v>
-      </c>
-      <c r="F19" s="5">
-        <v>49</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4">
-        <v>2006</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="4">
-        <v>10</v>
-      </c>
-      <c r="F20" s="5">
-        <v>50</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:8" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>8</v>
@@ -1181,19 +1357,21 @@
         <v>2006</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E21" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F21" s="5">
-        <v>51</v>
-      </c>
-      <c r="G21" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>8</v>
@@ -1205,37 +1383,41 @@
         <v>25</v>
       </c>
       <c r="E22" s="4">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <v>49</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="4">
         <v>5</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F23" s="5">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1">
-      <c r="A23" t="s">
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="1">
-        <v>2006</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="1">
-        <v>15</v>
-      </c>
-      <c r="F23" s="2">
-        <v>59</v>
-      </c>
-      <c r="G23"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -1244,204 +1426,231 @@
         <v>2006</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2">
+        <v>59</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2">
+        <v>71</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="4">
         <v>10</v>
       </c>
-      <c r="F24" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1">
-      <c r="A25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="F26" s="5">
+        <v>50</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4">
         <v>2006</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="1">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2">
-        <v>18</v>
-      </c>
-      <c r="G25"/>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2006</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="1">
-        <v>11</v>
-      </c>
-      <c r="F26" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="3" customFormat="1">
-      <c r="A27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2008</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1">
-        <v>9</v>
-      </c>
-      <c r="F27" s="2">
-        <v>22</v>
-      </c>
-      <c r="G27"/>
-      <c r="H27"/>
+      <c r="D27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="4">
+        <v>7</v>
+      </c>
+      <c r="F27" s="5">
+        <v>51</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1">
+        <v>9</v>
+      </c>
+      <c r="F28" s="2">
+        <v>22</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
         <v>2013</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1">
         <v>5</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <v>68</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="4">
-        <v>2007</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="4">
-        <v>6</v>
-      </c>
-      <c r="F29" s="5">
-        <v>53</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="3"/>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="6" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F30" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6</v>
+      </c>
+      <c r="F31" s="2">
+        <v>21</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="4">
         <v>2007</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="1">
-        <v>7</v>
-      </c>
-      <c r="F31" s="2">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2007</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="1">
-        <v>7</v>
-      </c>
-      <c r="F32" s="2">
-        <v>3</v>
-      </c>
+      <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4">
+        <v>6</v>
+      </c>
+      <c r="F32" s="5">
+        <v>53</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1</v>
+      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>57</v>
+      <c r="A33" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C33" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E33" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F33" s="2">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>55</v>
+      <c r="A34" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1450,18 +1659,21 @@
         <v>2006</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E34" s="1">
         <v>10</v>
       </c>
       <c r="F34" s="2">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>60</v>
+      <c r="A35" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1470,146 +1682,161 @@
         <v>2006</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F35" s="2">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="3" customFormat="1">
-      <c r="A36" t="s">
-        <v>56</v>
+      <c r="A36" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E36" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F36" s="2">
-        <v>63</v>
-      </c>
-      <c r="G36"/>
+        <v>16</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>59</v>
+      <c r="A37" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E37" s="1">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F37" s="2">
-        <v>37</v>
+        <v>62</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>58</v>
+      <c r="A38" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F38" s="2">
-        <v>40</v>
+        <v>3</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="3" customFormat="1">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E39" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F39" s="2">
-        <v>1</v>
-      </c>
-      <c r="G39"/>
+        <v>39</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
       <c r="H39"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4">
-        <v>2007</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="4">
-        <v>9</v>
-      </c>
-      <c r="F40" s="5">
-        <v>9</v>
-      </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="3"/>
+      <c r="E40" s="1">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2">
+        <v>45</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="4">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
         <v>2006</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="4">
-        <v>15</v>
-      </c>
-      <c r="F41" s="5">
-        <v>43</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6</v>
+      </c>
+      <c r="F41" s="2">
+        <v>38</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -1621,292 +1848,326 @@
         <v>20</v>
       </c>
       <c r="E42" s="1">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F42" s="2">
-        <v>36</v>
+        <v>63</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="3" customFormat="1">
-      <c r="A43" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="4">
-        <v>2012</v>
-      </c>
-      <c r="D43" s="4" t="s">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="4">
-        <v>7</v>
-      </c>
-      <c r="F43" s="5">
-        <v>25</v>
-      </c>
-      <c r="G43" s="5"/>
+      <c r="E43" s="1">
+        <v>15</v>
+      </c>
+      <c r="F43" s="2">
+        <v>37</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="1">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E44" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F44" s="2">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="G44" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="1">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E45" s="1">
+        <v>3</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2007</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="4">
+        <v>9</v>
+      </c>
+      <c r="F46" s="5">
+        <v>9</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="4">
+        <v>2006</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="4">
         <v>15</v>
       </c>
-      <c r="F45" s="2">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E46" s="1">
-        <v>9</v>
-      </c>
-      <c r="F46" s="2">
+      <c r="F47" s="5">
+        <v>43</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="1">
+        <v>23</v>
+      </c>
+      <c r="F48" s="2">
         <v>36</v>
       </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="1">
-        <v>15</v>
-      </c>
-      <c r="F47" s="2">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="4">
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="4">
         <v>2012</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E48" s="4">
-        <v>12</v>
-      </c>
-      <c r="F48" s="5">
-        <v>35</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" s="3" customFormat="1">
-      <c r="A49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2006</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E49" s="1">
-        <v>23</v>
-      </c>
-      <c r="F49" s="2">
-        <v>60</v>
-      </c>
-      <c r="G49"/>
-      <c r="H49"/>
+      <c r="D49" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="4">
+        <v>7</v>
+      </c>
+      <c r="F49" s="5">
+        <v>25</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="1">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E50" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F50" s="2">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="1">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E51" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F51" s="2">
-        <v>7</v>
+        <v>73</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="4">
-        <v>2013</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="4">
-        <v>4</v>
-      </c>
-      <c r="F52" s="3">
-        <v>33</v>
-      </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="1">
+        <v>9</v>
+      </c>
+      <c r="F52" s="2">
+        <v>54</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="4">
-        <v>2013</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="4">
-        <v>4</v>
-      </c>
-      <c r="F53" s="3">
-        <v>32</v>
-      </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="1">
+        <v>15</v>
+      </c>
+      <c r="F53" s="2">
+        <v>72</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:8" s="3" customFormat="1">
-      <c r="A54" t="s">
-        <v>30</v>
-      </c>
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2007</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="1">
-        <v>12</v>
-      </c>
-      <c r="F54" s="2">
-        <v>23</v>
-      </c>
-      <c r="G54"/>
-      <c r="H54"/>
+      <c r="A54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="4">
+        <v>2012</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="4">
+        <v>12</v>
+      </c>
+      <c r="F54" s="5">
+        <v>35</v>
+      </c>
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E55" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F55" s="2">
-        <v>44</v>
+        <v>60</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="3" customFormat="1">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>12</v>
@@ -1915,61 +2176,66 @@
         <v>12</v>
       </c>
       <c r="F56" s="2">
-        <v>34</v>
-      </c>
-      <c r="G56"/>
+        <v>74</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
       <c r="H56"/>
     </row>
     <row r="57" spans="1:8" s="3" customFormat="1">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F57" s="2">
-        <v>27</v>
-      </c>
-      <c r="G57"/>
+        <v>23</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1</v>
+      </c>
       <c r="H57"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="4">
-        <v>2013</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="4">
-        <v>2</v>
-      </c>
-      <c r="F58" s="5">
-        <v>29</v>
-      </c>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4</v>
+      </c>
+      <c r="F58" s="2">
+        <v>7</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C59" s="4">
         <v>2013</v>
@@ -1978,20 +2244,22 @@
         <v>12</v>
       </c>
       <c r="E59" s="4">
-        <v>3</v>
-      </c>
-      <c r="F59" s="5">
-        <v>26</v>
-      </c>
-      <c r="G59" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="F59" s="3">
+        <v>33</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1</v>
+      </c>
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C60" s="4">
         <v>2013</v>
@@ -2000,57 +2268,65 @@
         <v>12</v>
       </c>
       <c r="E60" s="4">
-        <v>2</v>
-      </c>
-      <c r="F60" s="5">
-        <v>28</v>
-      </c>
-      <c r="G60" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="F60" s="3">
+        <v>32</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C61" s="1">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E61" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F61" s="2">
-        <v>17</v>
+        <v>70</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C62" s="1">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" s="2">
-        <v>24</v>
+        <v>42</v>
+      </c>
+      <c r="G62" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:H62">
-    <sortCondition ref="B2:B62"/>
+    <sortCondition ref="A2:A62"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
table: which ones were used in analysis and why?
</commit_message>
<xml_diff>
--- a/data/publication_summary.xlsx
+++ b/data/publication_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12340" yWindow="0" windowWidth="12340" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="9800" yWindow="0" windowWidth="14920" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,6 +499,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -957,21 +960,21 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.1640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -999,118 +1002,130 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>52</v>
+      <c r="A2" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G2" s="8">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>50</v>
+      <c r="A3" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
       </c>
-      <c r="F3" s="1">
-        <v>7</v>
+      <c r="F3" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="8">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>72</v>
+      <c r="A4" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="8">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>18</v>
+      <c r="A5" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="8">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>32</v>
+      <c r="A6" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="8">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>80</v>
@@ -1118,13 +1133,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -1132,113 +1147,112 @@
       <c r="E7" s="1">
         <v>12</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>79</v>
+      <c r="F7" s="1">
+        <v>12</v>
       </c>
       <c r="G7" s="8">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="8">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2007</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3">
-        <v>9</v>
-      </c>
-      <c r="G8" s="8">
-        <v>9</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
     <row r="9" spans="1:8" s="2" customFormat="1">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2010</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="1">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="A9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="8">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="H9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2010</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="A10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G10" s="8">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2011</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="8">
-        <v>13</v>
+      <c r="A11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2013</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="12">
+        <v>28</v>
       </c>
       <c r="H11" t="s">
         <v>80</v>
@@ -1246,56 +1260,55 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9</v>
+      </c>
+      <c r="G12" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
         <v>2011</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G12" s="8">
-        <v>14</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
-      <c r="A13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2008</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1">
-        <v>13</v>
-      </c>
-      <c r="F13" s="1">
-        <v>13</v>
-      </c>
-      <c r="G13" s="8">
-        <v>16</v>
-      </c>
-      <c r="H13"/>
-    </row>
     <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
@@ -1321,354 +1334,355 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="4" t="s">
-        <v>71</v>
+      <c r="A15" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>2006</v>
+        <v>2010</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="1">
-        <v>3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G15" s="8">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="4" t="s">
-        <v>47</v>
+      <c r="A16" t="s">
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G16" s="8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3">
+        <v>9</v>
+      </c>
+      <c r="G17" s="8">
+        <v>30</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2008</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1">
-        <v>9</v>
-      </c>
-      <c r="F17" s="1">
-        <v>9</v>
-      </c>
-      <c r="G17" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G18" s="8">
-        <v>23</v>
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>79</v>
+        <v>18</v>
+      </c>
+      <c r="F19" s="1">
+        <v>18</v>
       </c>
       <c r="G19" s="8">
-        <v>24</v>
-      </c>
-      <c r="H19" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2012</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="3">
-        <v>7</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>79</v>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="1">
+        <v>13</v>
       </c>
       <c r="G20" s="8">
-        <v>25</v>
-      </c>
-      <c r="H20" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C21" s="3">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3">
-        <v>3</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>79</v>
+        <v>12</v>
+      </c>
+      <c r="F21" s="3">
+        <v>12</v>
       </c>
       <c r="G21" s="8">
-        <v>26</v>
-      </c>
-      <c r="H21" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="2" customFormat="1">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2013</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="A22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="3">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G22" s="8">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="2" customFormat="1">
-      <c r="A23" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="11">
-        <v>2013</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="11">
-        <v>2</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="12">
-        <v>28</v>
-      </c>
-      <c r="H23" t="s">
-        <v>80</v>
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="3">
+        <v>5</v>
+      </c>
+      <c r="F23" s="3">
+        <v>5</v>
+      </c>
+      <c r="G23" s="8">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3">
-        <v>2013</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3">
-        <v>2</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="A24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G24" s="8">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="H24" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="2" customFormat="1">
-      <c r="A25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2013</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="A25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="8">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="3">
+        <v>10</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="8">
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1">
+      <c r="A27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="3">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="8">
+        <v>51</v>
+      </c>
+      <c r="H27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1">
         <v>9</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F28" s="1">
         <v>9</v>
       </c>
-      <c r="G25" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2013</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="1">
-        <v>9</v>
-      </c>
-      <c r="F26" s="1">
-        <v>9</v>
-      </c>
-      <c r="G26" s="8">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="2" customFormat="1">
-      <c r="A27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="3">
-        <v>2013</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="3">
-        <v>4</v>
-      </c>
-      <c r="F27" s="3">
-        <v>4</v>
-      </c>
-      <c r="G27" s="9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="3">
-        <v>2013</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="3">
-        <v>4</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="9">
-        <v>33</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>77</v>
+      <c r="G28" s="8">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" t="s">
-        <v>14</v>
+      <c r="A29" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
         <v>2013</v>
@@ -1677,97 +1691,97 @@
         <v>12</v>
       </c>
       <c r="E29" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F29" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G29" s="8">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="3">
-        <v>2012</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="3">
-        <v>12</v>
-      </c>
-      <c r="F30" s="3">
-        <v>12</v>
+      <c r="A30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
       </c>
       <c r="G30" s="8">
-        <v>35</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>54</v>
+      <c r="A31" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E31" s="1">
+        <v>6</v>
+      </c>
+      <c r="F31" s="1">
+        <v>6</v>
+      </c>
+      <c r="G31" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2007</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="3">
+        <v>6</v>
+      </c>
+      <c r="F32" s="3">
+        <v>6</v>
+      </c>
+      <c r="G32" s="8">
+        <v>53</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="1">
-        <v>23</v>
-      </c>
-      <c r="G31" s="8">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2006</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="1">
-        <v>15</v>
-      </c>
-      <c r="F32" s="1">
-        <v>15</v>
-      </c>
-      <c r="G32" s="8">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" t="s">
-        <v>8</v>
-      </c>
       <c r="C33" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -1776,12 +1790,12 @@
         <v>6</v>
       </c>
       <c r="G33" s="8">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>57</v>
+      <c r="A34" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -1790,21 +1804,21 @@
         <v>2006</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E34" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34" s="8">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>58</v>
+      <c r="A35" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
@@ -1813,51 +1827,51 @@
         <v>2006</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E35" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G35" s="8">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="2" customFormat="1">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F36" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G36" s="8">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>75</v>
+      <c r="A37" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
@@ -1869,58 +1883,55 @@
         <v>7</v>
       </c>
       <c r="G37" s="8">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="3">
-        <v>2006</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="3">
-        <v>15</v>
-      </c>
-      <c r="F38" s="3">
-        <v>15</v>
+      <c r="A38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="1">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1">
+        <v>7</v>
       </c>
       <c r="G38" s="8">
-        <v>43</v>
-      </c>
-      <c r="H38" s="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:8" s="2" customFormat="1">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="1">
         <v>11</v>
       </c>
-      <c r="C39" s="1">
-        <v>2009</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="1">
-        <v>13</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>79</v>
+      <c r="F39" s="1">
+        <v>11</v>
       </c>
       <c r="G39" s="8">
-        <v>44</v>
-      </c>
-      <c r="H39" t="s">
-        <v>80</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H39"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
@@ -1949,134 +1960,127 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="3">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1">
         <v>2006</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="3">
-        <v>5</v>
-      </c>
-      <c r="F41" s="3">
-        <v>5</v>
+      <c r="D41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="1">
+        <v>6</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6</v>
       </c>
       <c r="G41" s="8">
-        <v>46</v>
-      </c>
-      <c r="H41" s="2"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="3">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1">
         <v>2006</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="3">
-        <v>12</v>
-      </c>
-      <c r="F42" s="3">
-        <v>12</v>
+      <c r="E42" s="1">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G42" s="8">
-        <v>47</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="H42" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:8" s="2" customFormat="1">
-      <c r="A43" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="3">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1">
         <v>2006</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E43" s="3">
-        <v>12</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>79</v>
+      <c r="D43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="1">
+        <v>15</v>
+      </c>
+      <c r="F43" s="1">
+        <v>15</v>
       </c>
       <c r="G43" s="8">
-        <v>49</v>
-      </c>
-      <c r="H43" t="s">
-        <v>80</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="H43"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="3">
+      <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1">
         <v>2006</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="3">
-        <v>10</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>79</v>
+      <c r="D44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1">
+        <v>4</v>
       </c>
       <c r="G44" s="8">
-        <v>50</v>
-      </c>
-      <c r="H44" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="3">
-        <v>2006</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="3">
-        <v>7</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>79</v>
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="1">
+        <v>3</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3</v>
       </c>
       <c r="G45" s="8">
-        <v>51</v>
-      </c>
-      <c r="H45" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="5" t="s">
-        <v>48</v>
+      <c r="A46" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>8</v>
@@ -2085,45 +2089,46 @@
         <v>2007</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E46" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F46" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G46" s="8">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E47" s="1">
-        <v>9</v>
-      </c>
-      <c r="F47" s="1">
-        <v>9</v>
+      <c r="A47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="3">
+        <v>2006</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="3">
+        <v>15</v>
+      </c>
+      <c r="F47" s="3">
+        <v>15</v>
       </c>
       <c r="G47" s="8">
+        <v>43</v>
+      </c>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -2132,39 +2137,39 @@
         <v>2006</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E48" s="1">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F48" s="1">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G48" s="8">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="2" customFormat="1">
-      <c r="A49" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2006</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="A49" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="3">
+        <v>7</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G49" s="8">
         <v>25</v>
-      </c>
-      <c r="E49" s="1">
-        <v>15</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G49" s="8">
-        <v>59</v>
       </c>
       <c r="H49" t="s">
         <v>80</v>
@@ -2172,301 +2177,299 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="1">
-        <v>2006</v>
+        <v>2013</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E50" s="1">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G50" s="8">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="H50" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="4" t="s">
-        <v>49</v>
+      <c r="A51" t="s">
+        <v>37</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="1">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E51" s="1">
-        <v>7</v>
-      </c>
-      <c r="F51" s="1">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G51" s="8">
-        <v>62</v>
+        <v>73</v>
+      </c>
+      <c r="H51" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E52" s="1">
-        <v>6</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>79</v>
+        <v>9</v>
+      </c>
+      <c r="F52" s="1">
+        <v>9</v>
       </c>
       <c r="G52" s="8">
-        <v>63</v>
-      </c>
-      <c r="H52" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="1">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E53" s="1">
-        <v>18</v>
-      </c>
-      <c r="F53" s="1">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G53" s="8">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="H53" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="2" customFormat="1">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="1">
-        <v>2008</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="1">
-        <v>13</v>
-      </c>
-      <c r="F54" s="1">
-        <v>13</v>
+      <c r="A54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="3">
+        <v>12</v>
+      </c>
+      <c r="F54" s="3">
+        <v>12</v>
       </c>
       <c r="G54" s="8">
-        <v>66</v>
-      </c>
-      <c r="H54"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="1">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E55" s="1">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G55" s="8">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H55" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="2" customFormat="1">
-      <c r="A56" s="4" t="s">
-        <v>27</v>
+      <c r="A56" t="s">
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="1">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F56" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G56" s="8">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H56"/>
     </row>
     <row r="57" spans="1:8" s="2" customFormat="1">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C57" s="1">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E57" s="1">
-        <v>13</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>79</v>
+        <v>12</v>
+      </c>
+      <c r="F57" s="1">
+        <v>12</v>
       </c>
       <c r="G57" s="8">
-        <v>69</v>
-      </c>
-      <c r="H57" t="s">
-        <v>80</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="H57"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C58" s="1">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G58" s="8">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="H58" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E59" s="1">
-        <v>8</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G59" s="8">
-        <v>71</v>
-      </c>
-      <c r="H59" t="s">
-        <v>80</v>
+      <c r="A59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="3">
+        <v>4</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G59" s="9">
+        <v>33</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="1">
-        <v>2005</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E60" s="1">
-        <v>15</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G60" s="8">
-        <v>72</v>
-      </c>
-      <c r="H60" t="s">
-        <v>80</v>
-      </c>
+      <c r="A60" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="3">
+        <v>2013</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="3">
+        <v>4</v>
+      </c>
+      <c r="F60" s="3">
+        <v>4</v>
+      </c>
+      <c r="G60" s="9">
+        <v>32</v>
+      </c>
+      <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C61" s="1">
         <v>2005</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E61" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G61" s="8">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H61" t="s">
         <v>80</v>
@@ -2474,10 +2477,10 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C62" s="1">
         <v>2006</v>
@@ -2486,18 +2489,18 @@
         <v>12</v>
       </c>
       <c r="E62" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G62" s="8">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:H62">
-    <sortCondition ref="G2:G62"/>
+    <sortCondition ref="A2:A62"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>